<commit_message>
experimenting with dax expressions
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\research\master-classes\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78A58E5-3862-4718-8EFC-AEC6CE3937D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F210C94B-424D-4030-BF34-FBF022C48F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -207,6 +207,54 @@
   </si>
   <si>
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/new_table_dax_scalar_tabular_329b1d08e3.mp4</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>1. Introduction to Python
+2. Applications of Python
+3. Bird's eye view of some popular packages
+4. Relevance to a Data Analyst/Engineer/Scientist</t>
+  </si>
+  <si>
+    <t>1. Programming basics : 
+a) variables
+b) loops
+c) functions</t>
+  </si>
+  <si>
+    <t>Data Structures : 
+1. Basic data types : int, float, string
+2. Complex data types : list, set, tuple, dict
+3. Classes</t>
+  </si>
+  <si>
+    <t>1. Data Ingestion with Python
+a) different types of files</t>
+  </si>
+  <si>
+    <t>Statistical Analysis with Python</t>
+  </si>
+  <si>
+    <t>Data Visualization with Python</t>
+  </si>
+  <si>
+    <t>Data Wrangling with Python</t>
+  </si>
+  <si>
+    <t>Data Processing with Python</t>
+  </si>
+  <si>
+    <t>Data Quality Checks with Python</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Walkthrough of Jupyter Notebooks
+a. Cells (code vs markdown)
+b. GUI way of adding cell, removing cell, moving cell up/down
+c. switching between code and markdown cell
+d. very high level markdown examples
+</t>
   </si>
 </sst>
 </file>
@@ -270,11 +318,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -590,21 +641,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="153.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="60.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="153.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -612,583 +664,708 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
         <v>49</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="B50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
         <v>56</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B60" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F691FC13-227C-4C95-87F3-82C0C38B24E7}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{2D275199-9484-474D-B5E6-D0465CF9EBE5}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{CD6A04B2-2DEA-4085-82D7-20B6B0FA8825}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{3DA293CC-6FDE-467E-939D-A58488637463}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{C40DCD9C-0844-4FF1-8062-27305941618D}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{F9F607EC-C2F0-40F2-83F8-0FC6BDD3761B}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{9741300D-C7DE-4BF9-B8FC-04EBF9152530}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{A1E18C35-C69F-4315-BFCB-F119B9EBF91A}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{00FC1561-98AD-47F7-BFD0-5CE4A1061533}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{F0F94FAD-F7AB-40CB-B6A2-92257A4D4093}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{F381F8C2-5323-44E4-A7E0-4BD4BEC657D0}"/>
-    <hyperlink ref="C13" r:id="rId12" xr:uid="{369ACC44-6B67-44AA-93AC-5C6B176A1635}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{411A927F-ACE5-40D4-946B-11456660B647}"/>
-    <hyperlink ref="C15" r:id="rId14" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
-    <hyperlink ref="C16" r:id="rId15" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
-    <hyperlink ref="C17" r:id="rId16" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
-    <hyperlink ref="C18" r:id="rId17" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
-    <hyperlink ref="C19" r:id="rId18" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
-    <hyperlink ref="C22" r:id="rId21" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
-    <hyperlink ref="C23" r:id="rId22" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
-    <hyperlink ref="C24" r:id="rId23" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
-    <hyperlink ref="C25" r:id="rId24" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
-    <hyperlink ref="C26" r:id="rId25" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
-    <hyperlink ref="C27" r:id="rId26" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
-    <hyperlink ref="C28" r:id="rId27" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
-    <hyperlink ref="C29" r:id="rId28" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
-    <hyperlink ref="C30" r:id="rId29" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
-    <hyperlink ref="C31" r:id="rId30" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
-    <hyperlink ref="C32" r:id="rId31" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
-    <hyperlink ref="C33" r:id="rId32" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
-    <hyperlink ref="C34" r:id="rId33" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
-    <hyperlink ref="C35" r:id="rId34" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
-    <hyperlink ref="C36" r:id="rId35" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
-    <hyperlink ref="C37" r:id="rId36" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
-    <hyperlink ref="C38" r:id="rId37" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
-    <hyperlink ref="C39" r:id="rId38" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
-    <hyperlink ref="C40" r:id="rId39" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
-    <hyperlink ref="C41" r:id="rId40" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
-    <hyperlink ref="C43" r:id="rId41" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
-    <hyperlink ref="C44" r:id="rId42" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
-    <hyperlink ref="C45" r:id="rId43" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
-    <hyperlink ref="C47" r:id="rId44" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
-    <hyperlink ref="C46" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
-    <hyperlink ref="C48" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
-    <hyperlink ref="C49" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{F691FC13-227C-4C95-87F3-82C0C38B24E7}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{2D275199-9484-474D-B5E6-D0465CF9EBE5}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{CD6A04B2-2DEA-4085-82D7-20B6B0FA8825}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{3DA293CC-6FDE-467E-939D-A58488637463}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{C40DCD9C-0844-4FF1-8062-27305941618D}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{F9F607EC-C2F0-40F2-83F8-0FC6BDD3761B}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{9741300D-C7DE-4BF9-B8FC-04EBF9152530}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{A1E18C35-C69F-4315-BFCB-F119B9EBF91A}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{00FC1561-98AD-47F7-BFD0-5CE4A1061533}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{F0F94FAD-F7AB-40CB-B6A2-92257A4D4093}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{F381F8C2-5323-44E4-A7E0-4BD4BEC657D0}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{369ACC44-6B67-44AA-93AC-5C6B176A1635}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{411A927F-ACE5-40D4-946B-11456660B647}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
+    <hyperlink ref="D23" r:id="rId22" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
+    <hyperlink ref="D25" r:id="rId24" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
+    <hyperlink ref="D26" r:id="rId25" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
+    <hyperlink ref="D27" r:id="rId26" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
+    <hyperlink ref="D29" r:id="rId28" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
+    <hyperlink ref="D30" r:id="rId29" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
+    <hyperlink ref="D31" r:id="rId30" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
+    <hyperlink ref="D32" r:id="rId31" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
+    <hyperlink ref="D33" r:id="rId32" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
+    <hyperlink ref="D34" r:id="rId33" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
+    <hyperlink ref="D35" r:id="rId34" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
+    <hyperlink ref="D36" r:id="rId35" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
+    <hyperlink ref="D37" r:id="rId36" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
+    <hyperlink ref="D38" r:id="rId37" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
+    <hyperlink ref="D39" r:id="rId38" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
+    <hyperlink ref="D40" r:id="rId39" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
+    <hyperlink ref="D41" r:id="rId40" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
+    <hyperlink ref="D52" r:id="rId41" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
+    <hyperlink ref="D53" r:id="rId42" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
+    <hyperlink ref="D54" r:id="rId43" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
+    <hyperlink ref="D56" r:id="rId44" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
+    <hyperlink ref="D55" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
+    <hyperlink ref="D57" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
+    <hyperlink ref="D58" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId48"/>

</xml_diff>

<commit_message>
added video link of python in excel file
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\research\master-classes\data-analyst-masterclass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUCHISMITA MALLICK\Python Master Class\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F210C94B-424D-4030-BF34-FBF022C48F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B533C3BF-99DB-4566-9168-62C083D55324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="learning-videos" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -255,6 +253,9 @@
 c. switching between code and markdown cell
 d. very high level markdown examples
 </t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/intro_jupyter_v2_58fbfc1e40.mp4</t>
   </si>
 </sst>
 </file>
@@ -318,13 +319,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -643,20 +647,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="153.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="153.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -670,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -681,7 +685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -692,7 +696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -703,7 +707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -714,7 +718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -725,7 +729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -736,7 +740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -747,7 +751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -758,7 +762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -769,7 +773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -780,7 +784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -791,7 +795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -802,7 +806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -813,7 +817,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -824,7 +828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -835,7 +839,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -846,7 +850,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -857,7 +861,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -868,7 +872,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -879,7 +883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -890,7 +894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -901,7 +905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -912,7 +916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -923,7 +927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -934,7 +938,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -945,7 +949,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -956,7 +960,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -967,7 +971,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -978,7 +982,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -989,7 +993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1000,7 +1004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1011,7 +1015,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1022,7 +1026,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1033,7 +1037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1044,7 +1048,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1055,7 +1059,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1066,7 +1070,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1077,7 +1081,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1088,7 +1092,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1099,7 +1103,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1110,7 +1114,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1121,7 +1125,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1131,8 +1135,11 @@
       <c r="C43" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D43" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1143,7 +1150,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1154,7 +1161,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1165,7 +1172,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1176,7 +1183,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1187,7 +1194,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1198,7 +1205,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1209,7 +1216,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1220,7 +1227,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1231,7 +1238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1242,7 +1249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1253,7 +1260,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1264,7 +1271,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1275,7 +1282,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -1286,7 +1293,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1297,22 +1304,22 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
         <v>49</v>
       </c>
@@ -1366,9 +1373,10 @@
     <hyperlink ref="D55" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
     <hyperlink ref="D57" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
     <hyperlink ref="D58" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
+    <hyperlink ref="D43" r:id="rId48" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId48"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -1378,7 +1386,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added work in progress files for vba recording
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUCHISMITA MALLICK\Python Master Class\data-analyst-masterclass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\research\master-classes\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B533C3BF-99DB-4566-9168-62C083D55324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34AE240-E4E4-4359-B09B-A81E21150EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="learning-videos" sheetId="1" r:id="rId1"/>
@@ -647,20 +647,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="153.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="153.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -674,7 +674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -685,7 +685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -696,7 +696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -707,7 +707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -718,7 +718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -729,7 +729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -740,7 +740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -751,7 +751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -762,7 +762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -773,7 +773,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -784,7 +784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -795,7 +795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -806,7 +806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -817,7 +817,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -828,7 +828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -839,7 +839,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -850,7 +850,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -861,7 +861,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -872,7 +872,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -883,7 +883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -894,7 +894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -905,7 +905,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -916,7 +916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -927,7 +927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -938,7 +938,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -949,7 +949,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -960,7 +960,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -971,7 +971,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -982,7 +982,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -993,7 +993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -1304,22 +1304,22 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B60" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B62" s="1" t="s">
         <v>49</v>
       </c>
@@ -1386,7 +1386,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the into_to_vba link in masterclass-video-index
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\research\master-classes\data-analyst-masterclass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34AE240-E4E4-4359-B09B-A81E21150EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10337AFD-5553-4C08-8A2A-7BBFD79FF392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="learning-videos" sheetId="1" r:id="rId1"/>
     <sheet name="activities-solution-videos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -256,6 +256,15 @@
   </si>
   <si>
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/intro_jupyter_v2_58fbfc1e40.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/Introduction_to_Macro_346730ca8a.mp4</t>
+  </si>
+  <si>
+    <t>Introduction and Basic Demo of Macro</t>
+  </si>
+  <si>
+    <t>absolute vs Relative cell referencing in Macro</t>
   </si>
 </sst>
 </file>
@@ -645,22 +654,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="153.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="153.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -674,7 +683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -685,7 +694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -696,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -707,7 +716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -718,7 +727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -729,7 +738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -740,7 +749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -751,7 +760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -762,7 +771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -773,7 +782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -784,7 +793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -795,7 +804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -806,7 +815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -817,510 +826,530 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
+      <c r="C15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="B26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="2" t="s">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="B34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="B36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="B39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="B40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="B41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="B42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+    <row r="44" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>41</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>49</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>50</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>51</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
-        <v>52</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B59" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>57</v>
+      </c>
       <c r="B60" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1339,41 +1368,41 @@
     <hyperlink ref="D12" r:id="rId11" xr:uid="{F381F8C2-5323-44E4-A7E0-4BD4BEC657D0}"/>
     <hyperlink ref="D13" r:id="rId12" xr:uid="{369ACC44-6B67-44AA-93AC-5C6B176A1635}"/>
     <hyperlink ref="D14" r:id="rId13" xr:uid="{411A927F-ACE5-40D4-946B-11456660B647}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
-    <hyperlink ref="D19" r:id="rId18" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
-    <hyperlink ref="D20" r:id="rId19" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
-    <hyperlink ref="D21" r:id="rId20" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
-    <hyperlink ref="D22" r:id="rId21" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
-    <hyperlink ref="D24" r:id="rId23" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
-    <hyperlink ref="D25" r:id="rId24" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
-    <hyperlink ref="D26" r:id="rId25" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
-    <hyperlink ref="D27" r:id="rId26" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
-    <hyperlink ref="D28" r:id="rId27" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
-    <hyperlink ref="D29" r:id="rId28" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
-    <hyperlink ref="D30" r:id="rId29" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
-    <hyperlink ref="D31" r:id="rId30" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
-    <hyperlink ref="D32" r:id="rId31" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
-    <hyperlink ref="D33" r:id="rId32" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
-    <hyperlink ref="D34" r:id="rId33" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
-    <hyperlink ref="D35" r:id="rId34" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
-    <hyperlink ref="D36" r:id="rId35" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
-    <hyperlink ref="D37" r:id="rId36" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
-    <hyperlink ref="D38" r:id="rId37" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
-    <hyperlink ref="D39" r:id="rId38" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
-    <hyperlink ref="D40" r:id="rId39" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
-    <hyperlink ref="D41" r:id="rId40" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
-    <hyperlink ref="D52" r:id="rId41" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
-    <hyperlink ref="D53" r:id="rId42" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
-    <hyperlink ref="D54" r:id="rId43" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
-    <hyperlink ref="D56" r:id="rId44" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
-    <hyperlink ref="D55" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
-    <hyperlink ref="D57" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
-    <hyperlink ref="D58" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
-    <hyperlink ref="D43" r:id="rId48" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
+    <hyperlink ref="D17" r:id="rId14" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
+    <hyperlink ref="D19" r:id="rId16" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
+    <hyperlink ref="D20" r:id="rId17" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
+    <hyperlink ref="D21" r:id="rId18" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
+    <hyperlink ref="D22" r:id="rId19" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
+    <hyperlink ref="D23" r:id="rId20" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
+    <hyperlink ref="D24" r:id="rId21" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
+    <hyperlink ref="D25" r:id="rId22" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
+    <hyperlink ref="D26" r:id="rId23" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
+    <hyperlink ref="D27" r:id="rId24" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
+    <hyperlink ref="D28" r:id="rId25" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
+    <hyperlink ref="D29" r:id="rId26" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
+    <hyperlink ref="D30" r:id="rId27" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
+    <hyperlink ref="D31" r:id="rId28" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
+    <hyperlink ref="D32" r:id="rId29" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
+    <hyperlink ref="D33" r:id="rId30" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
+    <hyperlink ref="D34" r:id="rId31" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
+    <hyperlink ref="D35" r:id="rId32" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
+    <hyperlink ref="D36" r:id="rId33" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
+    <hyperlink ref="D37" r:id="rId34" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
+    <hyperlink ref="D38" r:id="rId35" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
+    <hyperlink ref="D39" r:id="rId36" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
+    <hyperlink ref="D40" r:id="rId37" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
+    <hyperlink ref="D41" r:id="rId38" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
+    <hyperlink ref="D42" r:id="rId39" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
+    <hyperlink ref="D43" r:id="rId40" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
+    <hyperlink ref="D54" r:id="rId41" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
+    <hyperlink ref="D55" r:id="rId42" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
+    <hyperlink ref="D56" r:id="rId43" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
+    <hyperlink ref="D58" r:id="rId44" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
+    <hyperlink ref="D57" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
+    <hyperlink ref="D59" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
+    <hyperlink ref="D60" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
+    <hyperlink ref="D45" r:id="rId48" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId49"/>
@@ -1386,7 +1415,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the absolute_relative_cell_referencing video link in mastercalss-video-index file
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUCHISMITA MALLICK\Python Master Class\data-analyst-masterclass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9000CE1C-22E2-4965-B4B9-6B1310258800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5A5CDE-D339-4FC0-8F73-8934582991D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="learning-videos" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -258,9 +258,6 @@
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/intro_jupyter_v2_58fbfc1e40.mp4</t>
   </si>
   <si>
-    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/Introduction_to_Macro_346730ca8a.mp4</t>
-  </si>
-  <si>
     <t>Introduction and Basic Demo of Macro</t>
   </si>
   <si>
@@ -268,13 +265,16 @@
   </si>
   <si>
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/variable_v1_7b8288e721.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/absolute_relative_cell_referencing_f0074d5341.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +301,12 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Avenir Next LT Pro"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF292B2C"/>
+      <name val="Lato"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -331,7 +337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -345,6 +351,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -662,11 +669,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -832,25 +839,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D15" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1174,7 +1183,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43</v>
       </c>
@@ -1185,7 +1194,7 @@
         <v>59</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="57" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added video link of python loop in excel file
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\data-analyst-masterclass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUCHISMITA MALLICK\Python Master Class\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE777D6-E644-4A31-8496-510D906897FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75B814C-7FEC-4DCC-A764-3D22669619C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="learning-videos" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -267,20 +267,23 @@
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/absolute_relative_cell_referencing_f0074d5341.mp4</t>
   </si>
   <si>
-    <t xml:space="preserve">https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/variable_v1_7b8288e721.mp4   </t>
-  </si>
-  <si>
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/string_v2_af19c8cf3d.mp4</t>
   </si>
   <si>
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/absolute_relative_cell_referencing_7186b91472.mp4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/variable_v1_7b8288e721.mp4     </t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/loops_e5dae15d3c.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,12 +310,6 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Avenir Next LT Pro"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF292B2C"/>
-      <name val="Lato"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -343,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -357,7 +354,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -675,20 +671,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="153.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="5" max="5" width="147.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -702,7 +699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -713,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -724,7 +721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -735,7 +732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -746,7 +743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -757,7 +754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -768,7 +765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -779,7 +776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -790,7 +787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -801,7 +798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -812,7 +809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -823,7 +820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -834,7 +831,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -845,7 +842,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -856,7 +853,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -864,10 +861,10 @@
         <v>70</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -878,7 +875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -889,7 +886,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -900,7 +897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -911,7 +908,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -922,7 +919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -933,7 +930,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -944,7 +941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -955,7 +952,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -966,7 +963,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -977,7 +974,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -988,7 +985,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -999,7 +996,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1010,7 +1007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1021,7 +1018,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1032,7 +1029,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1043,7 +1040,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -1054,7 +1051,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>31</v>
       </c>
@@ -1065,7 +1062,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>32</v>
       </c>
@@ -1076,7 +1073,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>33</v>
       </c>
@@ -1087,7 +1084,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>34</v>
       </c>
@@ -1098,7 +1095,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>35</v>
       </c>
@@ -1109,7 +1106,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>36</v>
       </c>
@@ -1120,7 +1117,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>37</v>
       </c>
@@ -1131,7 +1128,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>38</v>
       </c>
@@ -1142,7 +1139,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>39</v>
       </c>
@@ -1153,7 +1150,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>40</v>
       </c>
@@ -1175,7 +1172,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>42</v>
       </c>
@@ -1189,7 +1186,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="61.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43</v>
       </c>
@@ -1200,11 +1197,13 @@
         <v>59</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>44</v>
       </c>
@@ -1215,7 +1214,7 @@
         <v>60</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
@@ -1229,7 +1228,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>46</v>
       </c>
@@ -1240,7 +1239,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>47</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>48</v>
       </c>
@@ -1262,7 +1261,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>49</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>50</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>51</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>52</v>
       </c>
@@ -1306,7 +1305,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>53</v>
       </c>
@@ -1317,7 +1316,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>54</v>
       </c>
@@ -1328,7 +1327,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>55</v>
       </c>
@@ -1339,7 +1338,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>56</v>
       </c>
@@ -1350,7 +1349,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>57</v>
       </c>
@@ -1361,22 +1360,22 @@
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
         <v>49</v>
       </c>
@@ -1435,9 +1434,10 @@
     <hyperlink ref="D47" r:id="rId50" xr:uid="{ED3658BA-1644-4FA3-BA52-6F7CEE02366A}"/>
     <hyperlink ref="D16" r:id="rId51" xr:uid="{E98FAC7F-4B24-4275-B421-982A8FE27E1B}"/>
     <hyperlink ref="D15" r:id="rId52" xr:uid="{31B78239-FAB3-4B28-8098-72D668F76472}"/>
+    <hyperlink ref="E46" r:id="rId53" xr:uid="{884ABEC8-C457-4852-89DF-0131C7EE608A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId53"/>
+  <pageSetup orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added vba_to_script video link
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHUCHISMITA MALLICK\Python Master Class\data-analyst-masterclass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75B814C-7FEC-4DCC-A764-3D22669619C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A1FE4B-9297-4FF7-A1E2-60FF4B17193E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="learning-videos" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/loops_e5dae15d3c.mp4</t>
+  </si>
+  <si>
+    <t>Introduction ro VBA</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/vba_basic_script_475f65923e.mp4</t>
   </si>
 </sst>
 </file>
@@ -669,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -865,504 +871,510 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
+      <c r="C17" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
+        <v>39</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>40</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="B44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="57" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+    <row r="45" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>41</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="57" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>50</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>51</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>57</v>
+      </c>
       <c r="B61" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1377,6 +1389,11 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B64" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1395,49 +1412,50 @@
     <hyperlink ref="D12" r:id="rId11" xr:uid="{F381F8C2-5323-44E4-A7E0-4BD4BEC657D0}"/>
     <hyperlink ref="D13" r:id="rId12" xr:uid="{369ACC44-6B67-44AA-93AC-5C6B176A1635}"/>
     <hyperlink ref="D14" r:id="rId13" xr:uid="{411A927F-ACE5-40D4-946B-11456660B647}"/>
-    <hyperlink ref="D17" r:id="rId14" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
-    <hyperlink ref="D18" r:id="rId15" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
-    <hyperlink ref="D19" r:id="rId16" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
-    <hyperlink ref="D20" r:id="rId17" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
-    <hyperlink ref="D21" r:id="rId18" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
-    <hyperlink ref="D22" r:id="rId19" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
-    <hyperlink ref="D23" r:id="rId20" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
-    <hyperlink ref="D24" r:id="rId21" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
-    <hyperlink ref="D25" r:id="rId22" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
-    <hyperlink ref="D26" r:id="rId23" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
-    <hyperlink ref="D27" r:id="rId24" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
-    <hyperlink ref="D28" r:id="rId25" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
-    <hyperlink ref="D29" r:id="rId26" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
-    <hyperlink ref="D30" r:id="rId27" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
-    <hyperlink ref="D31" r:id="rId28" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
-    <hyperlink ref="D32" r:id="rId29" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
-    <hyperlink ref="D33" r:id="rId30" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
-    <hyperlink ref="D34" r:id="rId31" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
-    <hyperlink ref="D35" r:id="rId32" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
-    <hyperlink ref="D36" r:id="rId33" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
-    <hyperlink ref="D37" r:id="rId34" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
-    <hyperlink ref="D38" r:id="rId35" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
-    <hyperlink ref="D39" r:id="rId36" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
-    <hyperlink ref="D40" r:id="rId37" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
-    <hyperlink ref="D41" r:id="rId38" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
-    <hyperlink ref="D42" r:id="rId39" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
-    <hyperlink ref="D43" r:id="rId40" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
-    <hyperlink ref="D54" r:id="rId41" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
-    <hyperlink ref="D55" r:id="rId42" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
-    <hyperlink ref="D56" r:id="rId43" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
-    <hyperlink ref="D58" r:id="rId44" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
-    <hyperlink ref="D57" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
-    <hyperlink ref="D59" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
-    <hyperlink ref="D60" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
-    <hyperlink ref="D45" r:id="rId48" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
-    <hyperlink ref="D46" r:id="rId49" xr:uid="{2D014933-159A-4357-ACE9-705C9A15E8BB}"/>
-    <hyperlink ref="D47" r:id="rId50" xr:uid="{ED3658BA-1644-4FA3-BA52-6F7CEE02366A}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
+    <hyperlink ref="D19" r:id="rId15" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
+    <hyperlink ref="D20" r:id="rId16" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
+    <hyperlink ref="D21" r:id="rId17" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
+    <hyperlink ref="D22" r:id="rId18" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
+    <hyperlink ref="D23" r:id="rId19" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
+    <hyperlink ref="D24" r:id="rId20" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
+    <hyperlink ref="D25" r:id="rId21" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
+    <hyperlink ref="D26" r:id="rId22" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
+    <hyperlink ref="D27" r:id="rId23" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
+    <hyperlink ref="D28" r:id="rId24" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
+    <hyperlink ref="D29" r:id="rId25" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
+    <hyperlink ref="D30" r:id="rId26" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
+    <hyperlink ref="D31" r:id="rId27" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
+    <hyperlink ref="D32" r:id="rId28" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
+    <hyperlink ref="D33" r:id="rId29" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
+    <hyperlink ref="D34" r:id="rId30" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
+    <hyperlink ref="D35" r:id="rId31" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
+    <hyperlink ref="D36" r:id="rId32" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
+    <hyperlink ref="D37" r:id="rId33" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
+    <hyperlink ref="D38" r:id="rId34" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
+    <hyperlink ref="D39" r:id="rId35" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
+    <hyperlink ref="D40" r:id="rId36" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
+    <hyperlink ref="D41" r:id="rId37" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
+    <hyperlink ref="D42" r:id="rId38" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
+    <hyperlink ref="D43" r:id="rId39" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
+    <hyperlink ref="D44" r:id="rId40" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
+    <hyperlink ref="D55" r:id="rId41" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
+    <hyperlink ref="D56" r:id="rId42" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
+    <hyperlink ref="D57" r:id="rId43" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
+    <hyperlink ref="D59" r:id="rId44" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
+    <hyperlink ref="D58" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
+    <hyperlink ref="D60" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
+    <hyperlink ref="D61" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
+    <hyperlink ref="D46" r:id="rId48" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
+    <hyperlink ref="D47" r:id="rId49" xr:uid="{2D014933-159A-4357-ACE9-705C9A15E8BB}"/>
+    <hyperlink ref="D48" r:id="rId50" xr:uid="{ED3658BA-1644-4FA3-BA52-6F7CEE02366A}"/>
     <hyperlink ref="D16" r:id="rId51" xr:uid="{E98FAC7F-4B24-4275-B421-982A8FE27E1B}"/>
     <hyperlink ref="D15" r:id="rId52" xr:uid="{31B78239-FAB3-4B28-8098-72D668F76472}"/>
-    <hyperlink ref="E46" r:id="rId53" xr:uid="{884ABEC8-C457-4852-89DF-0131C7EE608A}"/>
+    <hyperlink ref="E47" r:id="rId53" xr:uid="{884ABEC8-C457-4852-89DF-0131C7EE608A}"/>
+    <hyperlink ref="D17" r:id="rId54" xr:uid="{5030F25D-F870-4F7E-B635-34C58F9314BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId54"/>
+  <pageSetup orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added the subroutines, cell-referencing, object-properties-methods and variables video link to masterclass-index-file
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A1FE4B-9297-4FF7-A1E2-60FF4B17193E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88C2418-3EED-43EB-B7D8-61908A81A76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -270,9 +270,6 @@
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/string_v2_af19c8cf3d.mp4</t>
   </si>
   <si>
-    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/absolute_relative_cell_referencing_7186b91472.mp4</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/variable_v1_7b8288e721.mp4     </t>
   </si>
   <si>
@@ -283,6 +280,27 @@
   </si>
   <si>
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/vba_basic_script_475f65923e.mp4</t>
+  </si>
+  <si>
+    <t>Object, properties and methods</t>
+  </si>
+  <si>
+    <t>Subroutines</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/absolute_relative_cell_referencing_13a02bde11.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/private_public_subroutines_242327ee14.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/object_properties_methods_3fc8aa3c74.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/vba_variables_279f76a706.mp4</t>
   </si>
 </sst>
 </file>
@@ -675,13 +693,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
-  <dimension ref="A1:E65"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -691,7 +710,7 @@
     <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -705,7 +724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -716,7 +735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -727,7 +746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -738,7 +757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -749,7 +768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -760,7 +779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -771,7 +790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -782,7 +801,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -793,7 +812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -804,7 +823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -815,7 +834,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -826,7 +845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -837,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -848,7 +867,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -859,7 +878,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -867,533 +886,566 @@
         <v>70</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="D19" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>16</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
+      <c r="C20" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>16</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>18</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="B25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>19</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="B26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>20</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>21</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>22</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>23</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>24</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="2" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>24</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>25</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>26</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>27</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="B34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>28</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>29</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="B36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>30</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>31</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>32</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="B39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>33</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="B40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>34</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="B41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>35</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="B42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>36</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>37</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="B44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>38</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="B45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>39</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="B46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>40</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="B47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="57" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>41</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
-        <v>42</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="57" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>43</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="57" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>44</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C54" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>48</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>49</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>50</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>51</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>52</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>53</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>54</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>56</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>55</v>
+      </c>
       <c r="B62" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D62" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>56</v>
+      </c>
       <c r="B63" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D63" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>57</v>
+      </c>
       <c r="B64" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D64" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1412,55 +1464,59 @@
     <hyperlink ref="D12" r:id="rId11" xr:uid="{F381F8C2-5323-44E4-A7E0-4BD4BEC657D0}"/>
     <hyperlink ref="D13" r:id="rId12" xr:uid="{369ACC44-6B67-44AA-93AC-5C6B176A1635}"/>
     <hyperlink ref="D14" r:id="rId13" xr:uid="{411A927F-ACE5-40D4-946B-11456660B647}"/>
-    <hyperlink ref="D18" r:id="rId14" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
-    <hyperlink ref="D19" r:id="rId15" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
-    <hyperlink ref="D20" r:id="rId16" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
-    <hyperlink ref="D21" r:id="rId17" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
-    <hyperlink ref="D22" r:id="rId18" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
-    <hyperlink ref="D23" r:id="rId19" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
-    <hyperlink ref="D24" r:id="rId20" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
-    <hyperlink ref="D25" r:id="rId21" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
-    <hyperlink ref="D26" r:id="rId22" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
-    <hyperlink ref="D27" r:id="rId23" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
-    <hyperlink ref="D28" r:id="rId24" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
-    <hyperlink ref="D29" r:id="rId25" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
-    <hyperlink ref="D30" r:id="rId26" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
-    <hyperlink ref="D31" r:id="rId27" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
-    <hyperlink ref="D32" r:id="rId28" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
-    <hyperlink ref="D33" r:id="rId29" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
-    <hyperlink ref="D34" r:id="rId30" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
-    <hyperlink ref="D35" r:id="rId31" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
-    <hyperlink ref="D36" r:id="rId32" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
-    <hyperlink ref="D37" r:id="rId33" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
-    <hyperlink ref="D38" r:id="rId34" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
-    <hyperlink ref="D39" r:id="rId35" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
-    <hyperlink ref="D40" r:id="rId36" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
-    <hyperlink ref="D41" r:id="rId37" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
-    <hyperlink ref="D42" r:id="rId38" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
-    <hyperlink ref="D43" r:id="rId39" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
-    <hyperlink ref="D44" r:id="rId40" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
-    <hyperlink ref="D55" r:id="rId41" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
-    <hyperlink ref="D56" r:id="rId42" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
-    <hyperlink ref="D57" r:id="rId43" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
-    <hyperlink ref="D59" r:id="rId44" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
-    <hyperlink ref="D58" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
-    <hyperlink ref="D60" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
-    <hyperlink ref="D61" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
-    <hyperlink ref="D46" r:id="rId48" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
-    <hyperlink ref="D47" r:id="rId49" xr:uid="{2D014933-159A-4357-ACE9-705C9A15E8BB}"/>
-    <hyperlink ref="D48" r:id="rId50" xr:uid="{ED3658BA-1644-4FA3-BA52-6F7CEE02366A}"/>
-    <hyperlink ref="D16" r:id="rId51" xr:uid="{E98FAC7F-4B24-4275-B421-982A8FE27E1B}"/>
-    <hyperlink ref="D15" r:id="rId52" xr:uid="{31B78239-FAB3-4B28-8098-72D668F76472}"/>
-    <hyperlink ref="E47" r:id="rId53" xr:uid="{884ABEC8-C457-4852-89DF-0131C7EE608A}"/>
-    <hyperlink ref="D17" r:id="rId54" xr:uid="{5030F25D-F870-4F7E-B635-34C58F9314BF}"/>
+    <hyperlink ref="D21" r:id="rId14" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
+    <hyperlink ref="D22" r:id="rId15" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
+    <hyperlink ref="D23" r:id="rId16" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
+    <hyperlink ref="D24" r:id="rId17" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
+    <hyperlink ref="D25" r:id="rId18" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
+    <hyperlink ref="D26" r:id="rId19" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
+    <hyperlink ref="D27" r:id="rId20" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
+    <hyperlink ref="D28" r:id="rId21" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
+    <hyperlink ref="D29" r:id="rId22" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
+    <hyperlink ref="D30" r:id="rId23" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
+    <hyperlink ref="D31" r:id="rId24" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
+    <hyperlink ref="D32" r:id="rId25" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
+    <hyperlink ref="D33" r:id="rId26" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
+    <hyperlink ref="D34" r:id="rId27" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
+    <hyperlink ref="D35" r:id="rId28" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
+    <hyperlink ref="D36" r:id="rId29" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
+    <hyperlink ref="D37" r:id="rId30" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
+    <hyperlink ref="D38" r:id="rId31" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
+    <hyperlink ref="D39" r:id="rId32" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
+    <hyperlink ref="D40" r:id="rId33" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
+    <hyperlink ref="D41" r:id="rId34" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
+    <hyperlink ref="D42" r:id="rId35" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
+    <hyperlink ref="D43" r:id="rId36" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
+    <hyperlink ref="D44" r:id="rId37" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
+    <hyperlink ref="D45" r:id="rId38" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
+    <hyperlink ref="D46" r:id="rId39" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
+    <hyperlink ref="D47" r:id="rId40" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
+    <hyperlink ref="D58" r:id="rId41" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
+    <hyperlink ref="D59" r:id="rId42" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
+    <hyperlink ref="D60" r:id="rId43" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
+    <hyperlink ref="D62" r:id="rId44" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
+    <hyperlink ref="D61" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
+    <hyperlink ref="D63" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
+    <hyperlink ref="D64" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
+    <hyperlink ref="D49" r:id="rId48" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
+    <hyperlink ref="D50" r:id="rId49" xr:uid="{2D014933-159A-4357-ACE9-705C9A15E8BB}"/>
+    <hyperlink ref="D51" r:id="rId50" xr:uid="{ED3658BA-1644-4FA3-BA52-6F7CEE02366A}"/>
+    <hyperlink ref="D15" r:id="rId51" xr:uid="{31B78239-FAB3-4B28-8098-72D668F76472}"/>
+    <hyperlink ref="E50" r:id="rId52" xr:uid="{884ABEC8-C457-4852-89DF-0131C7EE608A}"/>
+    <hyperlink ref="D17" r:id="rId53" xr:uid="{5030F25D-F870-4F7E-B635-34C58F9314BF}"/>
+    <hyperlink ref="D16" r:id="rId54" xr:uid="{F7DFA587-4DFF-4455-BE48-CF2508F55051}"/>
+    <hyperlink ref="D18" r:id="rId55" xr:uid="{7E9F5376-7C57-4257-AA4B-5EA483C0C73A}"/>
+    <hyperlink ref="D19" r:id="rId56" xr:uid="{25720DD5-E925-4444-9327-70F8954063C6}"/>
+    <hyperlink ref="D20" r:id="rId57" xr:uid="{35C17EDC-6004-4BDB-A01C-0F34AC323B18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId55"/>
+  <pageSetup orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3667BA0-B39D-4C74-8A3D-CA2F8EDC061D}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Added the video link of conditional_statement, dialog_controls and Loops
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88C2418-3EED-43EB-B7D8-61908A81A76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831383C5-1DC6-46D1-B53A-982F547C361D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="91">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -301,6 +301,27 @@
   </si>
   <si>
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/vba_variables_279f76a706.mp4</t>
+  </si>
+  <si>
+    <t>Conditional Statements</t>
+  </si>
+  <si>
+    <t>Dialog_controls</t>
+  </si>
+  <si>
+    <t>Loops</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/Conditional_Statement_98333aea5e.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/msgbox_inputbox_dialogue_controls_e04be65db9.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/loops_for_next_for_each_4a60b97fff.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/Loop_do_while_do_until_51c1429323.mp4</t>
   </si>
 </sst>
 </file>
@@ -364,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -377,6 +398,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -694,23 +718,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="153.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="156" style="1" customWidth="1"/>
     <col min="5" max="5" width="147.5703125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -724,7 +748,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -735,7 +759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -746,7 +770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -757,7 +781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -768,7 +792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -779,7 +803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -790,7 +814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -801,7 +825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -812,7 +836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -823,7 +847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -834,7 +858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -845,7 +869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -856,7 +880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -867,7 +891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -878,7 +902,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -889,7 +913,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -900,7 +924,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -911,7 +935,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
@@ -922,7 +946,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
@@ -933,519 +957,555 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>23</v>
+      <c r="C21" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>15</v>
-      </c>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>16</v>
-      </c>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>17</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>18</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>19</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>20</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>21</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>22</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>23</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="B33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>24</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="2" t="s">
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>24</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>25</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>26</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="B36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>27</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>28</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>29</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="B39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>30</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="B40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>31</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="B41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>32</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="B42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>33</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>34</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="B44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>35</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="B45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>36</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="B46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>37</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="B47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>38</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="B48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>39</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="B49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>40</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="B50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+    <row r="51" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>41</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>42</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>43</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>44</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C57" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>48</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>49</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>50</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>51</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>52</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>53</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>54</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
         <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>56</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>55</v>
+      </c>
       <c r="B65" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D65" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>56</v>
+      </c>
       <c r="B66" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D66" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>57</v>
+      </c>
       <c r="B67" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D67" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1464,53 +1524,57 @@
     <hyperlink ref="D12" r:id="rId11" xr:uid="{F381F8C2-5323-44E4-A7E0-4BD4BEC657D0}"/>
     <hyperlink ref="D13" r:id="rId12" xr:uid="{369ACC44-6B67-44AA-93AC-5C6B176A1635}"/>
     <hyperlink ref="D14" r:id="rId13" xr:uid="{411A927F-ACE5-40D4-946B-11456660B647}"/>
-    <hyperlink ref="D21" r:id="rId14" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
-    <hyperlink ref="D22" r:id="rId15" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
-    <hyperlink ref="D23" r:id="rId16" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
-    <hyperlink ref="D24" r:id="rId17" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
-    <hyperlink ref="D25" r:id="rId18" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
-    <hyperlink ref="D26" r:id="rId19" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
-    <hyperlink ref="D27" r:id="rId20" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
-    <hyperlink ref="D28" r:id="rId21" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
-    <hyperlink ref="D29" r:id="rId22" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
-    <hyperlink ref="D30" r:id="rId23" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
-    <hyperlink ref="D31" r:id="rId24" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
-    <hyperlink ref="D32" r:id="rId25" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
-    <hyperlink ref="D33" r:id="rId26" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
-    <hyperlink ref="D34" r:id="rId27" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
-    <hyperlink ref="D35" r:id="rId28" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
-    <hyperlink ref="D36" r:id="rId29" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
-    <hyperlink ref="D37" r:id="rId30" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
-    <hyperlink ref="D38" r:id="rId31" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
-    <hyperlink ref="D39" r:id="rId32" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
-    <hyperlink ref="D40" r:id="rId33" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
-    <hyperlink ref="D41" r:id="rId34" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
-    <hyperlink ref="D42" r:id="rId35" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
-    <hyperlink ref="D43" r:id="rId36" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
-    <hyperlink ref="D44" r:id="rId37" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
-    <hyperlink ref="D45" r:id="rId38" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
-    <hyperlink ref="D46" r:id="rId39" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
-    <hyperlink ref="D47" r:id="rId40" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
-    <hyperlink ref="D58" r:id="rId41" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
-    <hyperlink ref="D59" r:id="rId42" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
-    <hyperlink ref="D60" r:id="rId43" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
-    <hyperlink ref="D62" r:id="rId44" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
-    <hyperlink ref="D61" r:id="rId45" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
-    <hyperlink ref="D63" r:id="rId46" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
-    <hyperlink ref="D64" r:id="rId47" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
-    <hyperlink ref="D49" r:id="rId48" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
-    <hyperlink ref="D50" r:id="rId49" xr:uid="{2D014933-159A-4357-ACE9-705C9A15E8BB}"/>
-    <hyperlink ref="D51" r:id="rId50" xr:uid="{ED3658BA-1644-4FA3-BA52-6F7CEE02366A}"/>
-    <hyperlink ref="D15" r:id="rId51" xr:uid="{31B78239-FAB3-4B28-8098-72D668F76472}"/>
-    <hyperlink ref="E50" r:id="rId52" xr:uid="{884ABEC8-C457-4852-89DF-0131C7EE608A}"/>
-    <hyperlink ref="D17" r:id="rId53" xr:uid="{5030F25D-F870-4F7E-B635-34C58F9314BF}"/>
-    <hyperlink ref="D16" r:id="rId54" xr:uid="{F7DFA587-4DFF-4455-BE48-CF2508F55051}"/>
-    <hyperlink ref="D18" r:id="rId55" xr:uid="{7E9F5376-7C57-4257-AA4B-5EA483C0C73A}"/>
-    <hyperlink ref="D19" r:id="rId56" xr:uid="{25720DD5-E925-4444-9327-70F8954063C6}"/>
-    <hyperlink ref="D20" r:id="rId57" xr:uid="{35C17EDC-6004-4BDB-A01C-0F34AC323B18}"/>
+    <hyperlink ref="D25" r:id="rId14" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
+    <hyperlink ref="D26" r:id="rId15" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
+    <hyperlink ref="D27" r:id="rId16" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
+    <hyperlink ref="D28" r:id="rId17" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
+    <hyperlink ref="D29" r:id="rId18" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
+    <hyperlink ref="D30" r:id="rId19" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
+    <hyperlink ref="D31" r:id="rId20" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
+    <hyperlink ref="D32" r:id="rId21" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
+    <hyperlink ref="D33" r:id="rId22" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
+    <hyperlink ref="D34" r:id="rId23" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
+    <hyperlink ref="D35" r:id="rId24" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
+    <hyperlink ref="D36" r:id="rId25" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
+    <hyperlink ref="D37" r:id="rId26" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
+    <hyperlink ref="D38" r:id="rId27" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
+    <hyperlink ref="D39" r:id="rId28" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
+    <hyperlink ref="D40" r:id="rId29" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
+    <hyperlink ref="D41" r:id="rId30" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
+    <hyperlink ref="D42" r:id="rId31" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
+    <hyperlink ref="D43" r:id="rId32" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
+    <hyperlink ref="D44" r:id="rId33" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
+    <hyperlink ref="D45" r:id="rId34" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
+    <hyperlink ref="D46" r:id="rId35" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
+    <hyperlink ref="D47" r:id="rId36" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
+    <hyperlink ref="D48" r:id="rId37" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
+    <hyperlink ref="D49" r:id="rId38" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
+    <hyperlink ref="D50" r:id="rId39" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
+    <hyperlink ref="D61" r:id="rId40" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
+    <hyperlink ref="D62" r:id="rId41" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
+    <hyperlink ref="D63" r:id="rId42" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
+    <hyperlink ref="D65" r:id="rId43" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
+    <hyperlink ref="D64" r:id="rId44" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
+    <hyperlink ref="D66" r:id="rId45" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
+    <hyperlink ref="D67" r:id="rId46" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
+    <hyperlink ref="D52" r:id="rId47" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
+    <hyperlink ref="D53" r:id="rId48" xr:uid="{2D014933-159A-4357-ACE9-705C9A15E8BB}"/>
+    <hyperlink ref="D54" r:id="rId49" xr:uid="{ED3658BA-1644-4FA3-BA52-6F7CEE02366A}"/>
+    <hyperlink ref="D15" r:id="rId50" xr:uid="{31B78239-FAB3-4B28-8098-72D668F76472}"/>
+    <hyperlink ref="E53" r:id="rId51" xr:uid="{884ABEC8-C457-4852-89DF-0131C7EE608A}"/>
+    <hyperlink ref="D17" r:id="rId52" xr:uid="{5030F25D-F870-4F7E-B635-34C58F9314BF}"/>
+    <hyperlink ref="D16" r:id="rId53" xr:uid="{F7DFA587-4DFF-4455-BE48-CF2508F55051}"/>
+    <hyperlink ref="D18" r:id="rId54" xr:uid="{7E9F5376-7C57-4257-AA4B-5EA483C0C73A}"/>
+    <hyperlink ref="D19" r:id="rId55" xr:uid="{25720DD5-E925-4444-9327-70F8954063C6}"/>
+    <hyperlink ref="D20" r:id="rId56" xr:uid="{35C17EDC-6004-4BDB-A01C-0F34AC323B18}"/>
+    <hyperlink ref="D21" r:id="rId57" xr:uid="{9B345338-6786-4B06-B104-78D20D8149E0}"/>
+    <hyperlink ref="D22" r:id="rId58" xr:uid="{6684630D-49B3-4414-8998-9162E074677A}"/>
+    <hyperlink ref="D24" r:id="rId59" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
+    <hyperlink ref="E23" r:id="rId60" xr:uid="{44FE9BF6-14AD-451D-AB0E-9C5DA769F0DF}"/>
+    <hyperlink ref="D23" r:id="rId61" xr:uid="{18A8DBF8-4753-4D97-8928-C56E165EDD95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId58"/>
+  <pageSetup orientation="portrait" r:id="rId62"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added remaining video links to the masterclass-video-index
</commit_message>
<xml_diff>
--- a/masterclass-video-index.xlsx
+++ b/masterclass-video-index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\data-analyst-masterclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831383C5-1DC6-46D1-B53A-982F547C361D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94394778-C42A-405D-9678-DEA8090044EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{2311AE42-6336-4CD2-8588-774CF306DAA6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="105">
   <si>
     <t>Sl.No.</t>
   </si>
@@ -322,6 +322,48 @@
   </si>
   <si>
     <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/Loop_do_while_do_until_51c1429323.mp4</t>
+  </si>
+  <si>
+    <t>Error-Debugging</t>
+  </si>
+  <si>
+    <t>Calling Subroutine With parameters</t>
+  </si>
+  <si>
+    <t>Custome Functions</t>
+  </si>
+  <si>
+    <t>User Form Controls</t>
+  </si>
+  <si>
+    <t>Multi-Dimensional Array</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/multi_dimensional_array_f1a30879bf.mp4</t>
+  </si>
+  <si>
+    <t>Inroduction to array and Static array</t>
+  </si>
+  <si>
+    <t>Dynamic Array</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/Introduction_to_array_static_array_55dc751dc8.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/Dynamic_Array_4ad40891b2.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/user_form_controls_2_e48135627a.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/custom_functions_55706a02ab.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/parameterized_subroutines_linking_with_button_0be408f3c1.mp4</t>
+  </si>
+  <si>
+    <t>https://mentorskool-platform-uploads.s3.ap-south-1.amazonaws.com/strapiUploads/imageAssets/error_debugging_dee59acad1.mp4</t>
   </si>
 </sst>
 </file>
@@ -400,7 +442,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -718,13 +760,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5496A81-63D5-42A0-BF99-B889FA38C433}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -734,7 +776,7 @@
     <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -748,7 +790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -759,7 +801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -770,7 +812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -781,7 +823,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -792,7 +834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -803,7 +845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -814,7 +856,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -825,7 +867,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -836,7 +878,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -847,7 +889,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -858,7 +900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -869,7 +911,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -880,7 +922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -891,7 +933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -902,7 +944,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
@@ -913,7 +955,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -924,7 +966,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
@@ -935,7 +977,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
@@ -946,7 +988,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
@@ -957,7 +999,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
@@ -968,7 +1010,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
@@ -989,523 +1031,607 @@
       <c r="D23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>14</v>
-      </c>
+    <row r="24" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>15</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>16</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>17</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>18</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>19</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="B36" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>20</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="B37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>21</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="B38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>22</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="B39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>23</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="B40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>24</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="2" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>24</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>25</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="B42" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>26</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>27</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="B44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>28</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="B45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>29</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="B46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>30</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="B47" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>31</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="B48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>32</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="B49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>33</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="B50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>34</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="B51" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>35</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="B52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>36</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="B53" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>37</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="B54" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>38</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="B55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>39</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="B56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>40</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="B57" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="57" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
+    <row r="58" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>41</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>42</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>43</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>44</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>45</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>46</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
-        <v>47</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
-        <v>48</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C60" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>44</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>45</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>46</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>47</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>48</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>49</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>50</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>51</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>52</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>53</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>54</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
-        <v>55</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
-        <v>56</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
-        <v>57</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D68" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>52</v>
+      </c>
       <c r="B69" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D69" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>53</v>
+      </c>
       <c r="B70" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D70" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>54</v>
+      </c>
       <c r="B71" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>55</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>56</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>57</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1524,44 +1650,44 @@
     <hyperlink ref="D12" r:id="rId11" xr:uid="{F381F8C2-5323-44E4-A7E0-4BD4BEC657D0}"/>
     <hyperlink ref="D13" r:id="rId12" xr:uid="{369ACC44-6B67-44AA-93AC-5C6B176A1635}"/>
     <hyperlink ref="D14" r:id="rId13" xr:uid="{411A927F-ACE5-40D4-946B-11456660B647}"/>
-    <hyperlink ref="D25" r:id="rId14" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
-    <hyperlink ref="D26" r:id="rId15" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
-    <hyperlink ref="D27" r:id="rId16" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
-    <hyperlink ref="D28" r:id="rId17" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
-    <hyperlink ref="D29" r:id="rId18" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
-    <hyperlink ref="D30" r:id="rId19" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
-    <hyperlink ref="D31" r:id="rId20" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
-    <hyperlink ref="D32" r:id="rId21" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
-    <hyperlink ref="D33" r:id="rId22" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
-    <hyperlink ref="D34" r:id="rId23" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
-    <hyperlink ref="D35" r:id="rId24" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
-    <hyperlink ref="D36" r:id="rId25" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
-    <hyperlink ref="D37" r:id="rId26" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
-    <hyperlink ref="D38" r:id="rId27" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
-    <hyperlink ref="D39" r:id="rId28" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
-    <hyperlink ref="D40" r:id="rId29" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
-    <hyperlink ref="D41" r:id="rId30" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
-    <hyperlink ref="D42" r:id="rId31" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
-    <hyperlink ref="D43" r:id="rId32" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
-    <hyperlink ref="D44" r:id="rId33" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
-    <hyperlink ref="D45" r:id="rId34" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
-    <hyperlink ref="D46" r:id="rId35" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
-    <hyperlink ref="D47" r:id="rId36" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
-    <hyperlink ref="D48" r:id="rId37" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
-    <hyperlink ref="D49" r:id="rId38" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
-    <hyperlink ref="D50" r:id="rId39" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
-    <hyperlink ref="D61" r:id="rId40" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
-    <hyperlink ref="D62" r:id="rId41" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
-    <hyperlink ref="D63" r:id="rId42" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
-    <hyperlink ref="D65" r:id="rId43" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
-    <hyperlink ref="D64" r:id="rId44" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
-    <hyperlink ref="D66" r:id="rId45" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
-    <hyperlink ref="D67" r:id="rId46" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
-    <hyperlink ref="D52" r:id="rId47" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
-    <hyperlink ref="D53" r:id="rId48" xr:uid="{2D014933-159A-4357-ACE9-705C9A15E8BB}"/>
-    <hyperlink ref="D54" r:id="rId49" xr:uid="{ED3658BA-1644-4FA3-BA52-6F7CEE02366A}"/>
+    <hyperlink ref="D32" r:id="rId14" xr:uid="{D1D40F44-8190-42A3-8F6E-318DCC102613}"/>
+    <hyperlink ref="D33" r:id="rId15" xr:uid="{39EF7AF5-9462-4D6F-BD41-1D8C81D45E0C}"/>
+    <hyperlink ref="D34" r:id="rId16" xr:uid="{862FA106-BEAB-482F-8478-C08FFFA9AF82}"/>
+    <hyperlink ref="D35" r:id="rId17" xr:uid="{F7345347-653F-4397-82E0-55EF03EB2D13}"/>
+    <hyperlink ref="D36" r:id="rId18" xr:uid="{B50B13E9-8E64-4240-A2BF-DCD65B08DD30}"/>
+    <hyperlink ref="D37" r:id="rId19" xr:uid="{526C128F-BB29-4208-88B3-13148DA98C13}"/>
+    <hyperlink ref="D38" r:id="rId20" xr:uid="{F09C47FA-2D2C-4B06-9576-B99BB04270BB}"/>
+    <hyperlink ref="D39" r:id="rId21" xr:uid="{99B8E892-B79B-4E5C-AAF2-F241A2777300}"/>
+    <hyperlink ref="D40" r:id="rId22" xr:uid="{4CF608B9-45D1-4C45-9597-1DDADAADD4E1}"/>
+    <hyperlink ref="D41" r:id="rId23" xr:uid="{94A4110C-8034-4824-93A2-6B7FF7BC915D}"/>
+    <hyperlink ref="D42" r:id="rId24" xr:uid="{DDEC47C8-4E1B-4455-9FDE-D0098E510062}"/>
+    <hyperlink ref="D43" r:id="rId25" xr:uid="{BE6768A1-AF8D-4808-8A69-AE725081B8B4}"/>
+    <hyperlink ref="D44" r:id="rId26" xr:uid="{D10DC4D9-CFB1-43C4-9778-637325C49091}"/>
+    <hyperlink ref="D45" r:id="rId27" xr:uid="{F61ADAD9-93E8-4BA7-9860-0D369BB39F4D}"/>
+    <hyperlink ref="D46" r:id="rId28" xr:uid="{0B2D81CC-FBFF-453E-8827-1C04A1B2A95E}"/>
+    <hyperlink ref="D47" r:id="rId29" xr:uid="{95F1DB4D-CBF0-481E-B124-549C98FD017D}"/>
+    <hyperlink ref="D48" r:id="rId30" xr:uid="{4C4CB74E-E01B-46EA-A69F-409F3A579E95}"/>
+    <hyperlink ref="D49" r:id="rId31" xr:uid="{66F3DCEF-E59D-4208-8901-279C62D86A6B}"/>
+    <hyperlink ref="D50" r:id="rId32" xr:uid="{8021A499-6CFE-4BDC-AF60-24C9B0431A8A}"/>
+    <hyperlink ref="D51" r:id="rId33" xr:uid="{D5D50CCD-A98C-4A04-97A4-B73DC6AEFAE5}"/>
+    <hyperlink ref="D52" r:id="rId34" xr:uid="{2F69477B-7C41-42CE-A487-333AE1913885}"/>
+    <hyperlink ref="D53" r:id="rId35" xr:uid="{341B6466-CCAC-4D46-94E6-935210C77769}"/>
+    <hyperlink ref="D54" r:id="rId36" xr:uid="{CC5DD783-E33A-4500-81F8-CFF47409E068}"/>
+    <hyperlink ref="D55" r:id="rId37" xr:uid="{B4A58ADB-84A2-4ABC-B845-E6BC0E3763F1}"/>
+    <hyperlink ref="D56" r:id="rId38" xr:uid="{74095B4C-6CF2-46BD-8621-ECD9E1135864}"/>
+    <hyperlink ref="D57" r:id="rId39" xr:uid="{B43BC82D-1EBA-4C74-B1B0-0ADD3F99650F}"/>
+    <hyperlink ref="D68" r:id="rId40" xr:uid="{F1F105FD-6036-439A-8EA1-A67FEA495636}"/>
+    <hyperlink ref="D69" r:id="rId41" xr:uid="{6606ECCD-1CE8-49D1-A984-2B6C9876F57D}"/>
+    <hyperlink ref="D70" r:id="rId42" xr:uid="{8CDC1C35-C095-45C9-BC29-34F61885A9B2}"/>
+    <hyperlink ref="D72" r:id="rId43" xr:uid="{2D0FFA85-7583-4EE2-8CAC-0851A7292033}"/>
+    <hyperlink ref="D71" r:id="rId44" xr:uid="{92FA9B4A-566D-4644-99C8-203809ED52A4}"/>
+    <hyperlink ref="D73" r:id="rId45" xr:uid="{153FEB21-3B34-4CB7-B7BD-EA455D341586}"/>
+    <hyperlink ref="D74" r:id="rId46" xr:uid="{C3A92468-9638-4F26-9D3E-3CBCCECC1A6D}"/>
+    <hyperlink ref="D59" r:id="rId47" xr:uid="{CB8072B1-5446-4ADB-AD84-82A4397D6E9A}"/>
+    <hyperlink ref="D60" r:id="rId48" xr:uid="{2D014933-159A-4357-ACE9-705C9A15E8BB}"/>
+    <hyperlink ref="D61" r:id="rId49" xr:uid="{ED3658BA-1644-4FA3-BA52-6F7CEE02366A}"/>
     <hyperlink ref="D15" r:id="rId50" xr:uid="{31B78239-FAB3-4B28-8098-72D668F76472}"/>
-    <hyperlink ref="E53" r:id="rId51" xr:uid="{884ABEC8-C457-4852-89DF-0131C7EE608A}"/>
+    <hyperlink ref="E60" r:id="rId51" xr:uid="{884ABEC8-C457-4852-89DF-0131C7EE608A}"/>
     <hyperlink ref="D17" r:id="rId52" xr:uid="{5030F25D-F870-4F7E-B635-34C58F9314BF}"/>
     <hyperlink ref="D16" r:id="rId53" xr:uid="{F7DFA587-4DFF-4455-BE48-CF2508F55051}"/>
     <hyperlink ref="D18" r:id="rId54" xr:uid="{7E9F5376-7C57-4257-AA4B-5EA483C0C73A}"/>
@@ -1569,12 +1695,19 @@
     <hyperlink ref="D20" r:id="rId56" xr:uid="{35C17EDC-6004-4BDB-A01C-0F34AC323B18}"/>
     <hyperlink ref="D21" r:id="rId57" xr:uid="{9B345338-6786-4B06-B104-78D20D8149E0}"/>
     <hyperlink ref="D22" r:id="rId58" xr:uid="{6684630D-49B3-4414-8998-9162E074677A}"/>
-    <hyperlink ref="D24" r:id="rId59" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
+    <hyperlink ref="D31" r:id="rId59" xr:uid="{0710E00B-8013-47D2-BFEB-F598ED4D7D41}"/>
     <hyperlink ref="E23" r:id="rId60" xr:uid="{44FE9BF6-14AD-451D-AB0E-9C5DA769F0DF}"/>
     <hyperlink ref="D23" r:id="rId61" xr:uid="{18A8DBF8-4753-4D97-8928-C56E165EDD95}"/>
+    <hyperlink ref="D30" r:id="rId62" xr:uid="{06E2B467-B6E6-4C08-9C97-B459E16A1CF8}"/>
+    <hyperlink ref="D28" r:id="rId63" xr:uid="{68C9A787-6E63-455E-9904-8F384295F18A}"/>
+    <hyperlink ref="D29" r:id="rId64" xr:uid="{33A6AE5D-AFB9-4B0C-B6A8-16D0F01F931A}"/>
+    <hyperlink ref="D27" r:id="rId65" xr:uid="{25BCED31-54CB-4A65-9AB8-4622C4975D41}"/>
+    <hyperlink ref="D26" r:id="rId66" xr:uid="{E6104B2C-65EA-4650-95C8-17A1383B3221}"/>
+    <hyperlink ref="D25" r:id="rId67" xr:uid="{86C4A428-A3CA-40D5-A506-9391E246914B}"/>
+    <hyperlink ref="D24" r:id="rId68" xr:uid="{0F160DAE-5BEA-465B-A0F9-E1BE1EF2912C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId62"/>
+  <pageSetup orientation="portrait" r:id="rId69"/>
 </worksheet>
 </file>
 

</xml_diff>